<commit_message>
Edits to data investigation
</commit_message>
<xml_diff>
--- a/src/a_place_for_salvador_allende_investigation.xlsx
+++ b/src/a_place_for_salvador_allende_investigation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GoGro\Desktop\Repos\a-place-for-salvador-allende\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89308406-0D13-4DBD-AADA-B5E2F8F45703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E7A8AD-56C8-4FE0-91BB-279E0420CA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14205,7 +14205,7 @@
   <dimension ref="A1:AO781"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B110" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A119" sqref="A119"/>

</xml_diff>